<commit_message>
updates to code after prepping walkthrough
</commit_message>
<xml_diff>
--- a/FunctionAppSolution/DataProcessingFunctions/ParseExcel/WatchedMovies.xlsx
+++ b/FunctionAppSolution/DataProcessingFunctions/ParseExcel/WatchedMovies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BusinessAndDevelopment\code\ACW\ACW-ParseExcelToCosmosDB\FunctionAppSolution\DataProcessingFunctions\DataProcessingFunctions\ParseExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\acw_work\FunctionAppStarter\DataProcessingFunctions\ParseExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2B1942-D764-40EB-B94E-BC1AEC4D63FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FAC20A-94FB-4143-BAEF-A80E85D6ECB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28935" yWindow="4125" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28875" yWindow="2685" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Title</t>
   </si>
@@ -88,6 +85,33 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>MovieId</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>d861be4a-de63-49ba-94e0-57486b060d90</t>
+  </si>
+  <si>
+    <t>bd7d27f8-2f3d-4044-8117-e9e71e351339</t>
+  </si>
+  <si>
+    <t>a7730d44-e048-4879-b571-a8a92a94c1be</t>
+  </si>
+  <si>
+    <t>de44443e-7c36-4a51-8101-be42d0b572a1</t>
+  </si>
+  <si>
+    <t>86ae4a99-30aa-42f3-bf6e-0d08e535ff7d</t>
+  </si>
+  <si>
+    <t>a264bd90-22d5-47b7-aefe-0f6df48de7a3</t>
+  </si>
+  <si>
+    <t>572eedce-7e46-4d32-915a-f07c529fed2d</t>
   </si>
 </sst>
 </file>
@@ -123,8 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -406,152 +429,177 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="F2">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>2002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>2003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>1986</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="E7">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="E8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8">
+      <c r="F8">
         <v>1989</v>
       </c>
     </row>

</xml_diff>